<commit_message>
add inner/outer London mapping, tweak chart dimensions
</commit_message>
<xml_diff>
--- a/INPUT/Sub_regional mapping.xlsx
+++ b/INPUT/Sub_regional mapping.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Labour Market Update R Project\CCLB MARKDOWN\INPUT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greaterlondonauthority.sharepoint.com/sites/S_IU_GLAEconomics/Shared Documents/General/Micro/Labour Market/Out of Work/03. R/INPUT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BC2757-CCA2-4284-AA84-FDF96C80783F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{26BC2757-CCA2-4284-AA84-FDF96C80783F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E4A6A0E-6868-423B-BFE6-E5D843ED2811}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="-16250" windowWidth="28800" windowHeight="15380" xr2:uid="{A25FC69E-99FE-41CB-BD1E-8693DB6E9C7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A25FC69E-99FE-41CB-BD1E-8693DB6E9C7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="Inner-Outer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
   <si>
     <t>London borough</t>
   </si>
@@ -150,13 +151,22 @@
   </si>
   <si>
     <t>Sutton</t>
+  </si>
+  <si>
+    <t>Outer</t>
+  </si>
+  <si>
+    <t>Inner</t>
+  </si>
+  <si>
+    <t>Inner/outer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +181,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -211,10 +234,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -223,9 +247,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{317EBD48-6801-45EF-8376-24B4144A67D3}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -537,284 +563,419 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38301F3A-0B14-49D0-A933-CF4A0EDDD440}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A2,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A3,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A4,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A5,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A6,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A7,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A8,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A9,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A10,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C11" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A11,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C12" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A12,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C13" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A13,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C14" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A14,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C15" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A15,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C16" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A16,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C17" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A17,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C18" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A18,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C19" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A19,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C20" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A20,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C21" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A21,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C22" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A22,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C23" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A23,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C24" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A24,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C25" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A25,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C26" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A26,'Inner-Outer'!A:A,0),2)</f>
+        <v>Inner</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C27" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A27,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C28" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A28,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C29" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A29,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C30" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A30,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C31" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A31,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C32" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A32,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C33" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A33,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>34</v>
+      </c>
+      <c r="C34" s="3" t="str">
+        <f>INDEX('Inner-Outer'!$A:$B,MATCH($A34,'Inner-Outer'!A:A,0),2)</f>
+        <v>Outer</v>
       </c>
     </row>
   </sheetData>
@@ -822,7 +983,300 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23D4321-7AA6-4499-B916-87B7442A1703}">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100535EDF9DD8DBB143AE8CD71BDB6B0E3B" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f6f28cdb5a9692a6c52c88c0d72e532e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9" xmlns:ns3="fd7425d0-09b7-49b7-b351-1ad2162dc0d7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d5bf8c08f73f601645ffb79004a62600" ns2:_="" ns3:_="">
     <xsd:import namespace="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9"/>
@@ -1059,19 +1513,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{643B4AC0-3468-4861-A664-309060549A2E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA860D4F-E6D9-4A82-9238-FDB2FCAF468F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6D7FF4-0C96-41FA-9806-3251CC71031B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F64C4F6-DFDD-433D-8AAB-CB12AE072997}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7fc9ebc1-6786-4aad-aee1-fdcde6e01ff9"/>
+    <ds:schemaRef ds:uri="fd7425d0-09b7-49b7-b351-1ad2162dc0d7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>